<commit_message>
Fixed formulas.  Don't have a test.
</commit_message>
<xml_diff>
--- a/testing_resources/xlsxtest003.xlsx
+++ b/testing_resources/xlsxtest003.xlsx
@@ -14,54 +14,14 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
-    <t>Attended</t>
-  </si>
-  <si>
-    <t>Roy</t>
-  </si>
-  <si>
-    <t>Wilkins</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Farmer</t>
-  </si>
-  <si>
-    <t>Ralph</t>
-  </si>
-  <si>
-    <t>Abernathy</t>
-  </si>
-  <si>
-    <t>Ella</t>
-  </si>
-  <si>
-    <t>Baker</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
   </numFmts>
   <fonts count="4">
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -123,9 +83,8 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -143,69 +102,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C4" activeCellId="0" pane="topLeft" sqref="C4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <f aca="false">A1+A2</f>
         <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>